<commit_message>
Grabs keywords, writes to KnownErrors text
However also writes to UnknownErrors text... need to fix. Grabs keywords
column from local Excel sheet
</commit_message>
<xml_diff>
--- a/Known_Install_log_Issues_.xlsx
+++ b/Known_Install_log_Issues_.xlsx
@@ -13,18 +13,18 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Mirza, Salman - Personal View" guid="{4FBB84C6-9885-482F-95BB-A4D3B60A7C11}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="807" activeSheetId="1"/>
+    <customWorkbookView name="Zou, Barry - Personal View" guid="{D46562BD-0088-43C4-8741-9EF109DEA2F5}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="1"/>
+    <customWorkbookView name="Newyear-Ramirez, Risa - Personal View" guid="{E72D1259-F149-4F4E-A740-5A269D6F9FB2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1902" windowHeight="837" activeSheetId="1"/>
+    <customWorkbookView name="Horikiri, Ren - Personal View" guid="{CF1E55BD-3305-4F8C-9024-CE58A53E137B}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1643" windowHeight="714" activeSheetId="1"/>
+    <customWorkbookView name="Xia, Jinshi - Personal View" guid="{0B2F7BD6-5279-43D0-936D-E78A7BBD42A7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
     <customWorkbookView name="Zhou, Jill - Personal View" guid="{2C3F5170-AB0E-47C9-B9CE-5BC568ADAEE7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="1"/>
-    <customWorkbookView name="Xia, Jinshi - Personal View" guid="{0B2F7BD6-5279-43D0-936D-E78A7BBD42A7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
-    <customWorkbookView name="Horikiri, Ren - Personal View" guid="{CF1E55BD-3305-4F8C-9024-CE58A53E137B}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1643" windowHeight="714" activeSheetId="1"/>
-    <customWorkbookView name="Newyear-Ramirez, Risa - Personal View" guid="{E72D1259-F149-4F4E-A740-5A269D6F9FB2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1902" windowHeight="837" activeSheetId="1"/>
-    <customWorkbookView name="Zou, Barry - Personal View" guid="{D46562BD-0088-43C4-8741-9EF109DEA2F5}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="1"/>
-    <customWorkbookView name="Mirza, Salman - Personal View" guid="{4FBB84C6-9885-482F-95BB-A4D3B60A7C11}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="807" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="152">
   <si>
     <t>Known error entries in setupengine.log that are False Positive/Not a problem</t>
   </si>
@@ -1099,6 +1099,18 @@
   </si>
   <si>
     <t>4.0SP10 FA</t>
+  </si>
+  <si>
+    <t>No property enclosed in raw argument brackets: []</t>
+  </si>
+  <si>
+    <t>10:31:09.010 Error: No property enclosed in raw argument brackets: []</t>
+  </si>
+  <si>
+    <t>This has no effect on product</t>
+  </si>
+  <si>
+    <t>1475_greatest</t>
   </si>
 </sst>
 </file>
@@ -1292,20 +1304,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="20" formatCode="d\-mmm\-yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="20" formatCode="d\-mmm\-yy"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" wrapText="1" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1316,7 +1315,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*" guid="{81BC102B-4386-441C-9BCC-A78F9902417C}" diskRevisions="1" revisionId="323" version="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{81CF74A1-5826-4093-9797-7CACD6DD92C1}" diskRevisions="1" revisionId="333" version="5">
   <header guid="{81BC102B-4386-441C-9BCC-A78F9902417C}" dateTime="2014-06-27T09:12:18" maxSheetId="4" userName="Zhou, Jill" r:id="rId56" minRId="313" maxRId="323">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -1324,7 +1323,83 @@
       <sheetId val="3"/>
     </sheetIdMap>
   </header>
+  <header guid="{4EAE2DF7-3697-49B3-AAC8-B87A0A5C01FD}" dateTime="2014-08-25T16:52:52" maxSheetId="4" userName="Newyear-Ramirez, Risa" r:id="rId57" minRId="324" maxRId="327">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{09B149ED-88CB-49AA-965D-C41E9A2F7514}" dateTime="2014-08-25T16:53:03" maxSheetId="4" userName="Newyear-Ramirez, Risa" r:id="rId58" minRId="328" maxRId="329">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{81CF74A1-5826-4093-9797-7CACD6DD92C1}" dateTime="2014-08-25T16:53:29" maxSheetId="4" userName="Newyear-Ramirez, Risa" r:id="rId59" minRId="330" maxRId="333">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
 </headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="324" sId="1" eol="1" ref="A29:XFD29" action="insertRow"/>
+  <rcc rId="325" sId="1">
+    <nc r="A29" t="inlineStr">
+      <is>
+        <t>No property enclosed in raw argument brackets: []</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="326" sId="1">
+    <nc r="B29" t="inlineStr">
+      <is>
+        <t>10:31:09.010 Error: No property enclosed in raw argument brackets: []</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="B29">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="327" sId="1">
+    <nc r="C29" t="inlineStr">
+      <is>
+        <t>This has no effect on product</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="328" sId="1">
+    <nc r="D29" t="inlineStr">
+      <is>
+        <t>Risa</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="329" sId="1" odxf="1" dxf="1" numFmtId="20">
+    <nc r="E29">
+      <v>41876</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="20" formatCode="d\-mmm\-yy"/>
+    </ndxf>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1439,9 +1514,43 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*" count="1">
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="330" sId="1">
+    <nc r="F29" t="inlineStr">
+      <is>
+        <t>miniBIP</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="331" sId="1">
+    <nc r="H29" t="inlineStr">
+      <is>
+        <t>Linux</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="332" sId="1">
+    <nc r="I29" t="inlineStr">
+      <is>
+        <t>Aurora_40_SP_REL</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="333" sId="1">
+    <nc r="J29" t="inlineStr">
+      <is>
+        <t>1475_greatest</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{81BC102B-4386-441C-9BCC-A78F9902417C}" name="Zou, Barry" id="-1742489466" dateTime="2014-06-26T12:01:56"/>
+  <userInfo guid="{81CF74A1-5826-4093-9797-7CACD6DD92C1}" name="Newyear-Ramirez, Risa" id="-2126829975" dateTime="2014-08-25T16:53:44"/>
 </users>
 </file>
 
@@ -1732,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,38 +2719,67 @@
         <v>1480</v>
       </c>
     </row>
+    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="14">
+        <v>41876</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2C3F5170-AB0E-47C9-B9CE-5BC568ADAEE7}" topLeftCell="A24">
-      <selection activeCell="C28" sqref="C28"/>
+    <customSheetView guid="{4FBB84C6-9885-482F-95BB-A4D3B60A7C11}" topLeftCell="C1">
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{D46562BD-0088-43C4-8741-9EF109DEA2F5}">
+      <selection activeCell="D9" sqref="D9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
+    </customSheetView>
+    <customSheetView guid="{E72D1259-F149-4F4E-A740-5A269D6F9FB2}">
+      <selection activeCell="B6" sqref="B6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
+    </customSheetView>
+    <customSheetView guid="{CF1E55BD-3305-4F8C-9024-CE58A53E137B}">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
     <customSheetView guid="{0B2F7BD6-5279-43D0-936D-E78A7BBD42A7}">
       <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{CF1E55BD-3305-4F8C-9024-CE58A53E137B}">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
-    </customSheetView>
-    <customSheetView guid="{E72D1259-F149-4F4E-A740-5A269D6F9FB2}">
-      <selection activeCell="B6" sqref="B6"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId4"/>
-    </customSheetView>
-    <customSheetView guid="{D46562BD-0088-43C4-8741-9EF109DEA2F5}">
-      <selection activeCell="D9" sqref="D9"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
     </customSheetView>
-    <customSheetView guid="{4FBB84C6-9885-482F-95BB-A4D3B60A7C11}" topLeftCell="C1">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+    <customSheetView guid="{2C3F5170-AB0E-47C9-B9CE-5BC568ADAEE7}" topLeftCell="A24">
+      <selection activeCell="C28" sqref="C28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId6"/>
     </customSheetView>
@@ -2660,22 +2798,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{2C3F5170-AB0E-47C9-B9CE-5BC568ADAEE7}">
+    <customSheetView guid="{4FBB84C6-9885-482F-95BB-A4D3B60A7C11}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{D46562BD-0088-43C4-8741-9EF109DEA2F5}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E72D1259-F149-4F4E-A740-5A269D6F9FB2}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CF1E55BD-3305-4F8C-9024-CE58A53E137B}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{0B2F7BD6-5279-43D0-936D-E78A7BBD42A7}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{CF1E55BD-3305-4F8C-9024-CE58A53E137B}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E72D1259-F149-4F4E-A740-5A269D6F9FB2}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{D46562BD-0088-43C4-8741-9EF109DEA2F5}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{4FBB84C6-9885-482F-95BB-A4D3B60A7C11}">
+    <customSheetView guid="{2C3F5170-AB0E-47C9-B9CE-5BC568ADAEE7}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -2692,22 +2830,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{2C3F5170-AB0E-47C9-B9CE-5BC568ADAEE7}">
+    <customSheetView guid="{4FBB84C6-9885-482F-95BB-A4D3B60A7C11}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{D46562BD-0088-43C4-8741-9EF109DEA2F5}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E72D1259-F149-4F4E-A740-5A269D6F9FB2}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CF1E55BD-3305-4F8C-9024-CE58A53E137B}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{0B2F7BD6-5279-43D0-936D-E78A7BBD42A7}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{CF1E55BD-3305-4F8C-9024-CE58A53E137B}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E72D1259-F149-4F4E-A740-5A269D6F9FB2}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{D46562BD-0088-43C4-8741-9EF109DEA2F5}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{4FBB84C6-9885-482F-95BB-A4D3B60A7C11}">
+    <customSheetView guid="{2C3F5170-AB0E-47C9-B9CE-5BC568ADAEE7}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>